<commit_message>
ActiPASS Version 1.43 Variable definitions
</commit_message>
<xml_diff>
--- a/Extra/ActiPASS_Variable-definitions_NewFormat_ActiPASS_Version_1.43.xlsx
+++ b/Extra/ActiPASS_Variable-definitions_NewFormat_ActiPASS_Version_1.43.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="200">
   <si>
     <t>varNames</t>
   </si>
@@ -908,13 +908,16 @@
   </si>
   <si>
     <t>"Run", "Cycle", "Stair", "Walk" with a cadence higher than 135/min , "Other" with periodic movement with a cadence higher than or equal to 135/min</t>
+  </si>
+  <si>
+    <t>ActiPASS Version 1.43 Variable Definitions</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -1006,6 +1009,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1038,7 +1049,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -1127,15 +1138,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyAlignment="1">
@@ -1219,10 +1240,15 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="5"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="5" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="20% - Accent2" xfId="3" builtinId="34"/>
     <cellStyle name="40% - Accent5" xfId="4" builtinId="47"/>
+    <cellStyle name="Heading 1" xfId="5" builtinId="16"/>
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="2" builtinId="10"/>
@@ -1503,10 +1529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C108"/>
+  <dimension ref="A1:C110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1515,903 +1541,911 @@
     <col min="2" max="3" width="79" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="18" thickBot="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" s="33" customFormat="1" ht="20.25" thickBot="1">
+      <c r="A1" s="33" t="s">
+        <v>199</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickTop="1"/>
+    <row r="3" spans="1:3" s="1" customFormat="1" ht="18" thickBot="1">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30.75" thickTop="1">
-      <c r="A2" t="s">
+    <row r="4" spans="1:3" ht="30.75" thickTop="1">
+      <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B4" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="30">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C3" s="4"/>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:3" ht="30">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C5" s="4"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" spans="1:3" ht="30">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B8" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" spans="1:3" s="11" customFormat="1" ht="30">
-      <c r="A7" s="11" t="s">
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" spans="1:3" s="11" customFormat="1" ht="30">
+      <c r="A9" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B9" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C9" s="11" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="11" customFormat="1" ht="30">
-      <c r="A8" s="11" t="s">
+    <row r="10" spans="1:3" s="11" customFormat="1" ht="30">
+      <c r="A10" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B10" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C10" s="11" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-    </row>
-    <row r="10" spans="1:3" s="19" customFormat="1" ht="60">
-      <c r="B10" s="21" t="s">
+    <row r="11" spans="1:3">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" spans="1:3" s="19" customFormat="1" ht="60">
+      <c r="B12" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="C10" s="20"/>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11" s="4"/>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" s="4"/>
+      <c r="C12" s="20"/>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:3" ht="30">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>84</v>
+        <v>52</v>
       </c>
       <c r="C14" s="4"/>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="4"/>
+    </row>
+    <row r="16" spans="1:3" ht="30">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" s="4"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B17" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="4"/>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
+      <c r="C17" s="4"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B18" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="4"/>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-    </row>
-    <row r="18" spans="1:3" s="15" customFormat="1" ht="90">
-      <c r="B18" s="18" t="s">
+      <c r="C18" s="4"/>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+    </row>
+    <row r="20" spans="1:3" s="15" customFormat="1" ht="90">
+      <c r="B20" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="C18" s="16"/>
-    </row>
-    <row r="19" spans="1:3" s="15" customFormat="1">
-      <c r="B19" s="17"/>
-      <c r="C19" s="16"/>
-    </row>
-    <row r="20" spans="1:3" s="5" customFormat="1" ht="91.5" customHeight="1">
-      <c r="B20" s="24" t="s">
+      <c r="C20" s="16"/>
+    </row>
+    <row r="21" spans="1:3" s="15" customFormat="1">
+      <c r="B21" s="17"/>
+      <c r="C21" s="16"/>
+    </row>
+    <row r="22" spans="1:3" s="5" customFormat="1" ht="91.5" customHeight="1">
+      <c r="B22" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="C20" s="6"/>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" s="4"/>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
-        <v>15</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C22" s="4"/>
+      <c r="C22" s="6"/>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" s="4"/>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" s="4"/>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B25" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C23" s="4"/>
-    </row>
-    <row r="24" spans="1:3" ht="30">
-      <c r="A24" t="s">
+      <c r="C25" s="4"/>
+    </row>
+    <row r="26" spans="1:3" ht="30">
+      <c r="A26" t="s">
         <v>92</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B26" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="C24" s="4"/>
-    </row>
-    <row r="25" spans="1:3" ht="30">
-      <c r="A25" t="s">
+      <c r="C26" s="4"/>
+    </row>
+    <row r="27" spans="1:3" ht="30">
+      <c r="A27" t="s">
         <v>93</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B27" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="C25" s="4"/>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="s">
+      <c r="C27" s="4"/>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
         <v>17</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B28" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C26" s="4"/>
-    </row>
-    <row r="27" spans="1:3" s="5" customFormat="1" ht="48.75" customHeight="1">
-      <c r="B27" s="24" t="s">
+      <c r="C28" s="4"/>
+    </row>
+    <row r="29" spans="1:3" s="5" customFormat="1" ht="48.75" customHeight="1">
+      <c r="B29" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="C27" s="6"/>
-    </row>
-    <row r="28" spans="1:3" ht="30">
-      <c r="A28" t="s">
-        <v>18</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="C28" s="10"/>
-    </row>
-    <row r="29" spans="1:3" ht="90">
-      <c r="A29" t="s">
-        <v>19</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="C29" s="10"/>
+      <c r="C29" s="6"/>
     </row>
     <row r="30" spans="1:3" ht="30">
       <c r="A30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C30" s="10"/>
+    </row>
+    <row r="31" spans="1:3" ht="90">
+      <c r="A31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C31" s="10"/>
+    </row>
+    <row r="32" spans="1:3" ht="30">
+      <c r="A32" t="s">
         <v>20</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B32" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="4"/>
-    </row>
-    <row r="31" spans="1:3" ht="30">
-      <c r="A31" t="s">
+      <c r="C32" s="4"/>
+    </row>
+    <row r="33" spans="1:3" ht="30">
+      <c r="A33" t="s">
         <v>21</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B33" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C31" s="4"/>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" t="s">
-        <v>22</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" s="5" customFormat="1" ht="54.75" customHeight="1">
-      <c r="B33" s="24" t="s">
-        <v>137</v>
-      </c>
-      <c r="C33" s="6"/>
+      <c r="C33" s="4"/>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" s="5" customFormat="1" ht="54.75" customHeight="1">
+      <c r="B35" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="C35" s="6"/>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
         <v>28</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B36" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="C34" s="4"/>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
-        <v>29</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C35" s="4"/>
-    </row>
-    <row r="36" spans="1:3" ht="30">
-      <c r="A36" t="s">
-        <v>30</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>69</v>
       </c>
       <c r="C36" s="4"/>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C37" s="4"/>
     </row>
-    <row r="38" spans="1:3" ht="45">
+    <row r="38" spans="1:3" ht="30">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="C38" s="4"/>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C39" s="4"/>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" ht="45">
       <c r="A40" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="C40" s="4"/>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>23</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>59</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C41" s="4"/>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>24</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>60</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C42" s="4"/>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>43</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C43" s="4"/>
-    </row>
-    <row r="44" spans="1:3" ht="30">
+        <v>23</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>44</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C44" s="4"/>
+        <v>24</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
+        <v>43</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C45" s="4"/>
+    </row>
+    <row r="46" spans="1:3" ht="30">
+      <c r="A46" t="s">
+        <v>44</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C46" s="4"/>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
         <v>45</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B47" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C45" s="4"/>
-    </row>
-    <row r="46" spans="1:3" ht="45.75" customHeight="1">
-      <c r="A46" t="s">
+      <c r="C47" s="4"/>
+    </row>
+    <row r="48" spans="1:3" ht="45.75" customHeight="1">
+      <c r="A48" t="s">
         <v>46</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B48" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C46" s="4"/>
-    </row>
-    <row r="47" spans="1:3" s="5" customFormat="1">
-      <c r="C47" s="23" t="s">
+      <c r="C48" s="4"/>
+    </row>
+    <row r="49" spans="1:3" s="5" customFormat="1">
+      <c r="C49" s="23" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="48" spans="1:3" s="5" customFormat="1">
-      <c r="B48" s="23" t="s">
+    <row r="50" spans="1:3" s="5" customFormat="1">
+      <c r="B50" s="23" t="s">
         <v>191</v>
       </c>
-      <c r="C48" s="5" t="s">
+      <c r="C50" s="5" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="90.75" thickBot="1">
-      <c r="A49" s="26" t="s">
+    <row r="51" spans="1:3" ht="90.75" thickBot="1">
+      <c r="A51" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="B49" s="27" t="s">
+      <c r="B51" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="C49" s="27" t="s">
+      <c r="C51" s="27" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="28" t="s">
+    <row r="52" spans="1:3">
+      <c r="A52" s="28" t="s">
         <v>175</v>
       </c>
-      <c r="B50" s="29" t="s">
+      <c r="B52" s="29" t="s">
         <v>176</v>
       </c>
-      <c r="C50" s="29" t="s">
+      <c r="C52" s="29" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="45">
-      <c r="A51" s="28" t="s">
+    <row r="53" spans="1:3" ht="45">
+      <c r="A53" s="28" t="s">
         <v>177</v>
       </c>
-      <c r="B51" s="29" t="s">
+      <c r="B53" s="29" t="s">
         <v>178</v>
       </c>
-      <c r="C51" s="29" t="s">
+      <c r="C53" s="29" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="45">
-      <c r="A52" s="28" t="s">
+    <row r="54" spans="1:3" ht="45">
+      <c r="A54" s="28" t="s">
         <v>179</v>
       </c>
-      <c r="B52" s="29" t="s">
+      <c r="B54" s="29" t="s">
         <v>180</v>
       </c>
-      <c r="C52" s="29" t="s">
+      <c r="C54" s="29" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="30">
-      <c r="A53" s="28" t="s">
+    <row r="55" spans="1:3" ht="30">
+      <c r="A55" s="28" t="s">
         <v>181</v>
       </c>
-      <c r="B53" s="29" t="s">
+      <c r="B55" s="29" t="s">
         <v>182</v>
       </c>
-      <c r="C53" s="29" t="s">
+      <c r="C55" s="29" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="30">
-      <c r="A54" s="28" t="s">
+    <row r="56" spans="1:3" ht="30">
+      <c r="A56" s="28" t="s">
         <v>186</v>
       </c>
-      <c r="B54" s="29" t="s">
+      <c r="B56" s="29" t="s">
         <v>187</v>
       </c>
-      <c r="C54" s="29" t="s">
+      <c r="C56" s="29" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="55" spans="1:3" s="5" customFormat="1">
-      <c r="A55" s="28" t="s">
+    <row r="57" spans="1:3" s="5" customFormat="1">
+      <c r="A57" s="28" t="s">
         <v>188</v>
       </c>
-      <c r="B55" s="29" t="s">
+      <c r="B57" s="29" t="s">
         <v>189</v>
       </c>
-      <c r="C55" s="29" t="s">
+      <c r="C57" s="29" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="56" spans="1:3" s="5" customFormat="1">
-      <c r="A56" s="28"/>
-      <c r="B56" s="29"/>
-      <c r="C56" s="29"/>
-    </row>
-    <row r="57" spans="1:3" s="5" customFormat="1">
-      <c r="B57" s="22" t="s">
+    <row r="58" spans="1:3" s="5" customFormat="1">
+      <c r="A58" s="28"/>
+      <c r="B58" s="29"/>
+      <c r="C58" s="29"/>
+    </row>
+    <row r="59" spans="1:3" s="5" customFormat="1">
+      <c r="B59" s="22" t="s">
         <v>98</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58" t="s">
-        <v>25</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="A59" t="s">
-        <v>26</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
+        <v>25</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
+        <v>26</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" t="s">
         <v>27</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B62" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="63" spans="1:3" s="5" customFormat="1" ht="120">
-      <c r="B63" s="13" t="s">
+    <row r="65" spans="1:3" s="5" customFormat="1" ht="120">
+      <c r="B65" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="C63" s="14" t="s">
+      <c r="C65" s="14" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
-      <c r="C64" s="30" t="s">
+    <row r="66" spans="1:3">
+      <c r="C66" s="30" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="A65" t="s">
-        <v>31</v>
-      </c>
-      <c r="B65" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C65" s="31"/>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66" t="s">
-        <v>32</v>
-      </c>
-      <c r="B66" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="C66" s="31"/>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C67" s="31"/>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C68" s="31"/>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>35</v>
-      </c>
-      <c r="B69" s="8" t="s">
-        <v>77</v>
+        <v>33</v>
+      </c>
+      <c r="B69" s="9" t="s">
+        <v>72</v>
       </c>
       <c r="C69" s="31"/>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>36</v>
-      </c>
-      <c r="B70" s="8" t="s">
-        <v>74</v>
+        <v>34</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>73</v>
       </c>
       <c r="C70" s="31"/>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
+        <v>35</v>
+      </c>
+      <c r="B71" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C71" s="31"/>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" t="s">
+        <v>36</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C72" s="31"/>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" t="s">
         <v>37</v>
       </c>
-      <c r="B71" s="7" t="s">
+      <c r="B73" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C71" s="31"/>
-    </row>
-    <row r="72" spans="1:3" ht="30">
-      <c r="A72" t="s">
+      <c r="C73" s="31"/>
+    </row>
+    <row r="74" spans="1:3" ht="30">
+      <c r="A74" t="s">
         <v>38</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B74" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C72" s="31"/>
-    </row>
-    <row r="75" spans="1:3" s="5" customFormat="1" ht="90">
-      <c r="B75" s="24" t="s">
+      <c r="C74" s="31"/>
+    </row>
+    <row r="77" spans="1:3" s="5" customFormat="1" ht="90">
+      <c r="B77" s="24" t="s">
         <v>193</v>
       </c>
-      <c r="C75" s="25" t="s">
+      <c r="C77" s="25" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="77" spans="1:3">
-      <c r="A77" t="s">
-        <v>142</v>
-      </c>
-      <c r="B77" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="C77" s="32" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3">
-      <c r="A78" t="s">
-        <v>143</v>
-      </c>
-      <c r="B78" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="C78" s="32"/>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B79" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="C79" s="32"/>
+        <v>103</v>
+      </c>
+      <c r="C79" s="32" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B80" s="10" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C80" s="32"/>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B81" s="10" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C81" s="32"/>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B82" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C82" s="32"/>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B83" s="10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C83" s="32"/>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B84" s="10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C84" s="32"/>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>157</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>111</v>
+        <v>148</v>
+      </c>
+      <c r="B85" s="10" t="s">
+        <v>109</v>
       </c>
       <c r="C85" s="32"/>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>150</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>112</v>
+        <v>149</v>
+      </c>
+      <c r="B86" s="10" t="s">
+        <v>110</v>
       </c>
       <c r="C86" s="32"/>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C87" s="32"/>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C88" s="32"/>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C89" s="32"/>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C90" s="32"/>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C91" s="32"/>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C92" s="32"/>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>158</v>
-      </c>
-      <c r="B93" s="10" t="s">
-        <v>119</v>
+        <v>155</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>117</v>
       </c>
       <c r="C93" s="32"/>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>159</v>
-      </c>
-      <c r="B94" s="10" t="s">
-        <v>120</v>
+        <v>156</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>118</v>
       </c>
       <c r="C94" s="32"/>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B95" s="10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C95" s="32"/>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B96" s="10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C96" s="32"/>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B97" s="10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C97" s="32"/>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B98" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C98" s="32"/>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B99" s="10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C99" s="32"/>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B100" s="10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C100" s="32"/>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>166</v>
-      </c>
-      <c r="B101" s="3" t="s">
-        <v>134</v>
+        <v>164</v>
+      </c>
+      <c r="B101" s="10" t="s">
+        <v>125</v>
       </c>
       <c r="C101" s="32"/>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>167</v>
-      </c>
-      <c r="B102" s="3" t="s">
-        <v>127</v>
+        <v>165</v>
+      </c>
+      <c r="B102" s="10" t="s">
+        <v>126</v>
       </c>
       <c r="C102" s="32"/>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="C103" s="32"/>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C104" s="32"/>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C105" s="32"/>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C106" s="32"/>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C107" s="32"/>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
+        <v>171</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C108" s="32"/>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" t="s">
+        <v>172</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C109" s="32"/>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110" t="s">
         <v>173</v>
       </c>
-      <c r="B108" s="3" t="s">
+      <c r="B110" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C108" s="32"/>
+      <c r="C110" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C64:C72"/>
-    <mergeCell ref="C77:C108"/>
+    <mergeCell ref="C66:C74"/>
+    <mergeCell ref="C79:C110"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>